<commit_message>
various labs tweasks, benchmark files,
</commit_message>
<xml_diff>
--- a/05-sql/Benchmarking_Dataformats.xlsx
+++ b/05-sql/Benchmarking_Dataformats.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sujee/ElephantScale/spark-labs/05-sql/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="23520" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
     <sheet name="sample results" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -20,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="12">
   <si>
     <t>parquet</t>
   </si>
@@ -53,6 +61,9 @@
   </si>
   <si>
     <t>size (GB)</t>
+  </si>
+  <si>
+    <t>Write Time</t>
   </si>
 </sst>
 </file>
@@ -154,7 +165,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -180,16 +191,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -202,6 +221,9 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -214,10 +236,18 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -257,7 +287,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$4</c:f>
+              <c:f>Sheet1!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -269,7 +299,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$A$7</c:f>
+              <c:f>Sheet1!$A$12:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -286,11 +316,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$7</c:f>
+              <c:f>Sheet1!$B$12:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
@@ -309,20 +342,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2130023288"/>
-        <c:axId val="2130026232"/>
+        <c:axId val="1500328256"/>
+        <c:axId val="1500332128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130023288"/>
+        <c:axId val="1500328256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130026232"/>
+        <c:crossAx val="1500332128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -330,7 +364,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130026232"/>
+        <c:axId val="1500332128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,7 +375,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130023288"/>
+        <c:crossAx val="1500328256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -385,7 +419,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$12:$A$14</c:f>
+              <c:f>Sheet1!$A$19:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -402,11 +436,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$B$14</c:f>
+              <c:f>Sheet1!$B$19:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
@@ -425,20 +462,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2130103304"/>
-        <c:axId val="2130106248"/>
+        <c:axId val="1500470688"/>
+        <c:axId val="1500474560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130103304"/>
+        <c:axId val="1500470688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130106248"/>
+        <c:crossAx val="1500474560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -446,7 +484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130106248"/>
+        <c:axId val="1500474560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,7 +495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130103304"/>
+        <c:crossAx val="1500470688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -500,7 +538,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$19</c:f>
+              <c:f>Sheet1!$C$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -512,7 +550,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$20:$A$23</c:f>
+              <c:f>Sheet1!$A$27:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -529,7 +567,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$23</c:f>
+              <c:f>Sheet1!$C$27:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -555,20 +593,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2129833144"/>
-        <c:axId val="2129836088"/>
+        <c:axId val="1508916112"/>
+        <c:axId val="1508945344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2129833144"/>
+        <c:axId val="1508916112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129836088"/>
+        <c:crossAx val="1508945344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -576,7 +615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2129836088"/>
+        <c:axId val="1508945344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,7 +626,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129833144"/>
+        <c:crossAx val="1508916112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -605,6 +644,251 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time (secs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>json</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>compressed json</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>parquet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1524878864"/>
+        <c:axId val="1524879392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1524878864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1524879392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1524879392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1524878864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -692,20 +976,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2129849928"/>
-        <c:axId val="2130165096"/>
+        <c:axId val="1504868304"/>
+        <c:axId val="1498449344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2129849928"/>
+        <c:axId val="1504868304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130165096"/>
+        <c:crossAx val="1498449344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -713,7 +998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130165096"/>
+        <c:axId val="1498449344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -724,7 +1009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129849928"/>
+        <c:crossAx val="1504868304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -741,7 +1026,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -808,20 +1093,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2130720280"/>
-        <c:axId val="2130723224"/>
+        <c:axId val="1497107968"/>
+        <c:axId val="1508080784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130720280"/>
+        <c:axId val="1497107968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130723224"/>
+        <c:crossAx val="1508080784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -829,7 +1115,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130723224"/>
+        <c:axId val="1508080784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,7 +1126,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130720280"/>
+        <c:crossAx val="1497107968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -857,7 +1143,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -938,20 +1224,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2131295736"/>
-        <c:axId val="2086800584"/>
+        <c:axId val="1497122720"/>
+        <c:axId val="1497248160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2131295736"/>
+        <c:axId val="1497122720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086800584"/>
+        <c:crossAx val="1497248160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -959,7 +1246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086800584"/>
+        <c:axId val="1497248160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -970,7 +1257,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131295736"/>
+        <c:crossAx val="1497122720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -987,20 +1274,563 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>770470</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:colOff>804336</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>135468</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>220135</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>67733</xdr:rowOff>
+      <xdr:colOff>254001</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1023,13 +1853,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>25399</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>262466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>338666</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1053,13 +1883,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>16933</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>110066</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1074,6 +1904,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>16933</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>8467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>143932</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1505,59 +2365,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D22"/>
+  <dimension ref="A2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="23">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B6" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="25">
-      <c r="A10" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1565,7 +2436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1573,13 +2444,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1587,67 +2460,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="25">
-      <c r="A18" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
+    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20" s="5">
         <v>0</v>
       </c>
-      <c r="C20">
-        <f>B20/1000000</f>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>0</v>
       </c>
-      <c r="D20">
-        <f>B20/1000000000</f>
+      <c r="B21" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
+    <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>B27/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>B27/1000000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21">
-        <f t="shared" ref="C21:C22" si="0">B21/1000000</f>
+      <c r="B28" s="5">
         <v>0</v>
       </c>
-      <c r="D21">
-        <f t="shared" ref="D21:D22" si="1">B21/1000000000</f>
+      <c r="C28">
+        <f t="shared" ref="C28:C29" si="0">B28/1000000</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
+      <c r="D28">
+        <f t="shared" ref="D28:D29" si="1">B28/1000000000</f>
         <v>0</v>
       </c>
-      <c r="B22" s="5">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>0</v>
       </c>
-      <c r="C22">
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+      <c r="C29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D22">
+      <c r="D29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1656,11 +2568,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1668,22 +2575,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="23">
+    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1691,7 +2598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1699,13 +2606,13 @@
         <v>39.431100000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1713,12 +2620,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="25">
+    <row r="10" spans="1:2" ht="26" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1726,7 +2633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1734,13 +2641,13 @@
         <v>25.78</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1748,12 +2655,12 @@
         <v>2.5920000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="25">
+    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1767,7 +2674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1783,7 +2690,7 @@
         <v>1.415188092</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1797,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1817,10 +2724,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sql labs updated for spark 2
</commit_message>
<xml_diff>
--- a/05-sql/Benchmarking_Dataformats.xlsx
+++ b/05-sql/Benchmarking_Dataformats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="23520" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="27900" windowHeight="18500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
   <si>
     <t>parquet</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Write Time</t>
+  </si>
+  <si>
+    <t>ORC</t>
+  </si>
+  <si>
+    <t>Data size</t>
   </si>
 </sst>
 </file>
@@ -165,8 +171,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -208,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -224,6 +254,18 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -239,6 +281,18 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -287,7 +341,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$11</c:f>
+              <c:f>Sheet1!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -299,9 +353,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$12:$A$14</c:f>
+              <c:f>Sheet1!$A$4:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>json</c:v>
                 </c:pt>
@@ -310,16 +364,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>parquet</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ORC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$B$14</c:f>
+              <c:f>Sheet1!$B$4:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -327,6 +384,9 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -342,11 +402,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1931705024"/>
-        <c:axId val="-1931701440"/>
+        <c:axId val="-65164912"/>
+        <c:axId val="-65162592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1931705024"/>
+        <c:axId val="-65164912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,7 +416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1931701440"/>
+        <c:crossAx val="-65162592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -364,7 +424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1931701440"/>
+        <c:axId val="-65162592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -375,7 +435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1931705024"/>
+        <c:crossAx val="-65164912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -419,9 +479,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$19:$A$21</c:f>
+              <c:f>Sheet1!$A$11:$A$14</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>json</c:v>
                 </c:pt>
@@ -430,16 +490,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>parquet</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ORC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$21</c:f>
+              <c:f>Sheet1!$B$11:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -447,6 +510,9 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -462,11 +528,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1931665600"/>
-        <c:axId val="-1931661728"/>
+        <c:axId val="-195417952"/>
+        <c:axId val="-195408256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1931665600"/>
+        <c:axId val="-195417952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -476,7 +542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1931661728"/>
+        <c:crossAx val="-195408256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -484,7 +550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1931661728"/>
+        <c:axId val="-195408256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1931665600"/>
+        <c:crossAx val="-195417952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -552,7 +618,7 @@
             <c:strRef>
               <c:f>Sheet1!$A$27:$A$30</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>json</c:v>
                 </c:pt>
@@ -561,6 +627,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>parquet</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ORC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -578,6 +647,9 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -593,11 +665,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1931624928"/>
-        <c:axId val="-1931621056"/>
+        <c:axId val="-195379696"/>
+        <c:axId val="-195370720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1931624928"/>
+        <c:axId val="-195379696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -607,7 +679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1931621056"/>
+        <c:crossAx val="-195370720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -615,7 +687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1931621056"/>
+        <c:axId val="-195370720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,7 +698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1931624928"/>
+        <c:crossAx val="-195379696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -669,7 +741,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$3</c:f>
+              <c:f>Sheet1!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -690,9 +762,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$19:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>json</c:v>
                 </c:pt>
@@ -701,16 +773,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>parquet</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ORC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$6</c:f>
+              <c:f>Sheet1!$B$19:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -718,6 +793,9 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -734,11 +812,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1931553040"/>
-        <c:axId val="-1931548400"/>
+        <c:axId val="-195337696"/>
+        <c:axId val="-195335376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1931553040"/>
+        <c:axId val="-195337696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -781,7 +859,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1931548400"/>
+        <c:crossAx val="-195335376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -789,7 +867,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1931548400"/>
+        <c:axId val="-195335376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +917,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1931553040"/>
+        <c:crossAx val="-195337696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -936,9 +1014,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'sample results'!$A$5:$A$7</c:f>
+              <c:f>'sample results'!$A$5:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>json</c:v>
                 </c:pt>
@@ -947,20 +1025,29 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>parquet</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ORC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'sample results'!$B$5:$B$7</c:f>
+              <c:f>'sample results'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>39.4311</c:v>
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -976,11 +1063,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1945351104"/>
-        <c:axId val="-1931590704"/>
+        <c:axId val="-67053344"/>
+        <c:axId val="-67012784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1945351104"/>
+        <c:axId val="-67053344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +1077,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1931590704"/>
+        <c:crossAx val="-67012784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -998,7 +1085,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1931590704"/>
+        <c:axId val="-67012784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,7 +1096,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1945351104"/>
+        <c:crossAx val="-67053344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1053,9 +1140,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'sample results'!$A$12:$A$14</c:f>
+              <c:f>'sample results'!$A$13:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>json</c:v>
                 </c:pt>
@@ -1064,21 +1151,30 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>parquet</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ORC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'sample results'!$B$12:$B$14</c:f>
+              <c:f>'sample results'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>25.78</c:v>
+                  <c:v>4.66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.592</c:v>
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1093,11 +1189,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1931528944"/>
-        <c:axId val="-1931525024"/>
+        <c:axId val="-60554656"/>
+        <c:axId val="-60552336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1931528944"/>
+        <c:axId val="-60554656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,7 +1203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1931525024"/>
+        <c:crossAx val="-60552336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1115,7 +1211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1931525024"/>
+        <c:axId val="-60552336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1126,7 +1222,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1931528944"/>
+        <c:crossAx val="-60554656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1169,7 +1265,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'sample results'!$C$19</c:f>
+              <c:f>'sample results'!$C$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1181,9 +1277,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'sample results'!$A$20:$A$23</c:f>
+              <c:f>'sample results'!$A$27:$A$30</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>json</c:v>
                 </c:pt>
@@ -1192,24 +1288,30 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>parquet</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ORC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'sample results'!$C$20:$C$23</c:f>
+              <c:f>'sample results'!$C$27:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1415.188092</c:v>
+                  <c:v>1415.178847</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>161.398938</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.667991</c:v>
+                  <c:v>118.394196</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105.793926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1224,11 +1326,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1930423424"/>
-        <c:axId val="-1930419504"/>
+        <c:axId val="-60534160"/>
+        <c:axId val="-60531840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1930423424"/>
+        <c:axId val="-60534160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1238,7 +1340,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1930419504"/>
+        <c:crossAx val="-60531840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1246,7 +1348,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1930419504"/>
+        <c:axId val="-60531840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1257,7 +1359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1930423424"/>
+        <c:crossAx val="-60534160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1269,6 +1371,232 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'sample results'!$A$21:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>parquet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ORC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'sample results'!$B$21:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>13.96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-57982416"/>
+        <c:axId val="-57980640"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-57982416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-57980640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-57980640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-57982416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1314,6 +1642,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1817,20 +2185,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>804336</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>135468</xdr:rowOff>
+      <xdr:colOff>753534</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>254001</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>601132</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1852,15 +2723,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>25399</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>262466</xdr:rowOff>
+      <xdr:colOff>8466</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>338666</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:colOff>321733</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>143935</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1912,14 +2783,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>16933</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>8467</xdr:rowOff>
+      <xdr:colOff>33865</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:colOff>330199</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>143932</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1954,7 +2825,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>220135</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>67733</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1978,16 +2849,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>25399</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>262466</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>8466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>338666</xdr:colOff>
+      <xdr:colOff>296333</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2012,13 +2883,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>16933</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>110066</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2035,6 +2906,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>59266</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2365,10 +3266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D29"/>
+  <dimension ref="A2:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2379,7 +3280,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2415,30 +3316,37 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -2446,7 +3354,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B13" s="5">
         <v>0</v>
@@ -2454,15 +3362,18 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>6</v>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="17" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2497,6 +3408,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="7"/>
+    </row>
     <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>7</v>
@@ -2561,6 +3486,22 @@
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30" si="2">B30/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30" si="3">B30/1000000000</f>
         <v>0</v>
       </c>
     </row>
@@ -2573,10 +3514,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D22"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2585,6 +3526,11 @@
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
@@ -2603,121 +3549,191 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>39.431100000000001</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5">
+        <v>5.25</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="5">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="26" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:2" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="5">
-        <v>25.78</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B13" s="5">
+        <v>4.66</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5">
+        <v>4.1100000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="5">
-        <v>2.5920000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B15" s="5">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="5">
-        <v>1415188092</v>
-      </c>
-      <c r="C20">
-        <f>B20/1000000</f>
-        <v>1415.1880920000001</v>
-      </c>
-      <c r="D20">
-        <f>B20/1000000000</f>
-        <v>1.415188092</v>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21">
-        <f t="shared" ref="C21:C22" si="0">B21/1000000</f>
         <v>0</v>
       </c>
-      <c r="D21">
-        <f t="shared" ref="D21:D22" si="1">B21/1000000000</f>
-        <v>0</v>
+      <c r="B21" s="5">
+        <v>13.96</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="5">
+        <v>18.59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+    </row>
+    <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1415178847</v>
+      </c>
+      <c r="C27">
+        <f>B27/1000000</f>
+        <v>1415.1788469999999</v>
+      </c>
+      <c r="D27">
+        <f>B27/1000000000</f>
+        <v>1.415178847</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="5">
+        <v>161398938</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:C29" si="0">B28/1000000</f>
+        <v>161.39893799999999</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28:D29" si="1">B28/1000000000</f>
+        <v>0.16139893799999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="5">
-        <v>80667991</v>
-      </c>
-      <c r="C22">
+      <c r="B29" s="5">
+        <v>118394196</v>
+      </c>
+      <c r="C29">
         <f t="shared" si="0"/>
-        <v>80.667991000000001</v>
-      </c>
-      <c r="D22">
+        <v>118.39419599999999</v>
+      </c>
+      <c r="D29">
         <f t="shared" si="1"/>
-        <v>8.0667990999999994E-2</v>
+        <v>0.11839419599999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="5">
+        <v>105793926</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30" si="2">B30/1000000</f>
+        <v>105.793926</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30" si="3">B30/1000000000</f>
+        <v>0.105793926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>